<commit_message>
Corrector kind of working
Can simulate 100,000s of years, but, Earth orbit unstable over large timescales
</commit_message>
<xml_diff>
--- a/Gantt Chart - RP.xlsx
+++ b/Gantt Chart - RP.xlsx
@@ -598,11 +598,11 @@
         </c:dLbls>
         <c:gapWidth val="41"/>
         <c:overlap val="100"/>
-        <c:axId val="2077588112"/>
-        <c:axId val="2077590160"/>
+        <c:axId val="2124417952"/>
+        <c:axId val="2124419728"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2077588112"/>
+        <c:axId val="2124417952"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -660,7 +660,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2077590160"/>
+        <c:crossAx val="2124419728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -668,7 +668,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2077590160"/>
+        <c:axId val="2124419728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="44050.0"/>
@@ -727,7 +727,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2077588112"/>
+        <c:crossAx val="2124417952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="60.0"/>
@@ -1325,13 +1325,13 @@
       <xdr:col>5</xdr:col>
       <xdr:colOff>229680</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>148616</xdr:rowOff>
+      <xdr:rowOff>148617</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>216173</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>40531</xdr:rowOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>27022</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>

</xml_diff>